<commit_message>
Extended the script with support for Buildings and Areas
</commit_message>
<xml_diff>
--- a/data/infrastructure.xlsx
+++ b/data/infrastructure.xlsx
@@ -1,23 +1,25 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matthijssenef\PycharmProjects\excel-2-esdl\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EACA66F8-5ECD-44A9-A7B9-875BCC1F57E5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88B4C749-824A-4F6F-B7A1-F2143CBDD36F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7620" yWindow="4815" windowWidth="19110" windowHeight="6315" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10680" yWindow="3435" windowWidth="38700" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Carriers" sheetId="3" r:id="rId1"/>
-    <sheet name="ConsumerProducer" sheetId="1" r:id="rId2"/>
-    <sheet name="Conversion" sheetId="4" r:id="rId3"/>
-    <sheet name="Transport" sheetId="5" r:id="rId4"/>
-    <sheet name="CablesPipesConnections" sheetId="2" r:id="rId5"/>
+    <sheet name="Areas" sheetId="6" r:id="rId1"/>
+    <sheet name="Buildings" sheetId="7" r:id="rId2"/>
+    <sheet name="Carriers" sheetId="3" r:id="rId3"/>
+    <sheet name="ConsumerProducer" sheetId="1" r:id="rId4"/>
+    <sheet name="Conversion" sheetId="4" r:id="rId5"/>
+    <sheet name="Transport" sheetId="5" r:id="rId6"/>
+    <sheet name="CablesPipesConnections" sheetId="2" r:id="rId7"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -29,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="78">
   <si>
     <t>ID</t>
   </si>
@@ -248,6 +250,21 @@
   </si>
   <si>
     <t>InPort2_Carrier</t>
+  </si>
+  <si>
+    <t>Scope</t>
+  </si>
+  <si>
+    <t>Parent_Area_ID</t>
+  </si>
+  <si>
+    <t>TopLevelArea</t>
+  </si>
+  <si>
+    <t>AreaBld_ID</t>
+  </si>
+  <si>
+    <t>Area_WKT</t>
   </si>
 </sst>
 </file>
@@ -288,7 +305,7 @@
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -565,10 +582,86 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AFEC4E92-53F5-402E-96D4-F7619F5A0534}">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.28515625" customWidth="1"/>
+    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>75</v>
+      </c>
+      <c r="D1" t="s">
+        <v>73</v>
+      </c>
+      <c r="E1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F1" t="s">
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E02B5F3F-629A-438E-A6DA-7E796848847B}">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="5" width="12.7109375" customWidth="1"/>
+    <col min="6" max="6" width="15" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" t="s">
+        <v>74</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6BEDCC5-740C-44C0-8CDC-4CA8E0BDF066}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -625,9 +718,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:L4"/>
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -635,16 +728,17 @@
   <cols>
     <col min="2" max="3" width="18.140625" customWidth="1"/>
     <col min="4" max="4" width="9.85546875" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125" customWidth="1"/>
-    <col min="7" max="7" width="11" customWidth="1"/>
-    <col min="8" max="8" width="11.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.5703125" customWidth="1"/>
+    <col min="8" max="8" width="11" customWidth="1"/>
+    <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -661,28 +755,31 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G1" t="s">
         <v>13</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>20</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>69</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>21</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>24</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>22</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>27</v>
       </c>
@@ -698,29 +795,32 @@
       <c r="E2">
         <v>4.51</v>
       </c>
-      <c r="F2">
+      <c r="F2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2">
         <v>10000</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>30</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>33</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>35</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>34</v>
       </c>
-      <c r="K2">
+      <c r="L2">
         <v>50</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>37</v>
       </c>
@@ -736,29 +836,32 @@
       <c r="E3">
         <v>4.51</v>
       </c>
-      <c r="F3">
+      <c r="F3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G3">
         <v>10000</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>41</v>
       </c>
-      <c r="H3" t="s">
+      <c r="I3" t="s">
         <v>6</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>40</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>34</v>
       </c>
-      <c r="K3">
+      <c r="L3">
         <v>20</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>60</v>
       </c>
@@ -774,18 +877,18 @@
       <c r="E4">
         <v>4.47</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4" t="s">
+        <v>48</v>
+      </c>
+      <c r="G4" s="1">
         <v>1000000000</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>62</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>7</v>
       </c>
-      <c r="I4" t="s">
-        <v>48</v>
-      </c>
       <c r="J4" t="s">
         <v>48</v>
       </c>
@@ -793,6 +896,9 @@
         <v>48</v>
       </c>
       <c r="L4" t="s">
+        <v>48</v>
+      </c>
+      <c r="M4" t="s">
         <v>48</v>
       </c>
     </row>
@@ -801,9 +907,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{37E59E50-3AA1-4991-AB07-24A7E9585BA0}">
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:Q3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -811,19 +917,20 @@
   <cols>
     <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="20.5703125" customWidth="1"/>
-    <col min="7" max="7" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="16.140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -840,40 +947,43 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G1" t="s">
         <v>13</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>15</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>14</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>16</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>71</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>17</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>72</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>18</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>11</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>19</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>42</v>
       </c>
@@ -889,41 +999,44 @@
       <c r="E2">
         <v>4.5</v>
       </c>
-      <c r="F2">
+      <c r="F2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2">
         <v>4000</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>45</v>
       </c>
-      <c r="H2">
+      <c r="I2">
         <v>3.2</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>46</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>6</v>
       </c>
-      <c r="K2" t="s">
-        <v>48</v>
-      </c>
       <c r="L2" t="s">
         <v>48</v>
       </c>
       <c r="M2" t="s">
+        <v>48</v>
+      </c>
+      <c r="N2" t="s">
         <v>47</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>33</v>
       </c>
-      <c r="O2" t="s">
-        <v>48</v>
-      </c>
       <c r="P2" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="Q2" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>54</v>
       </c>
@@ -939,37 +1052,40 @@
       <c r="E3">
         <v>4.4800000000000004</v>
       </c>
-      <c r="F3" s="1">
+      <c r="F3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G3" s="1">
         <v>1000000000</v>
       </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
         <v>57</v>
       </c>
-      <c r="H3">
+      <c r="I3">
         <v>0.4</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>58</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>7</v>
       </c>
-      <c r="K3" t="s">
-        <v>48</v>
-      </c>
       <c r="L3" t="s">
         <v>48</v>
       </c>
       <c r="M3" t="s">
+        <v>48</v>
+      </c>
+      <c r="N3" t="s">
         <v>59</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>6</v>
       </c>
-      <c r="O3" t="s">
-        <v>48</v>
-      </c>
       <c r="P3" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q3" t="s">
         <v>48</v>
       </c>
     </row>
@@ -978,9 +1094,9 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BD7264C-2E9E-4A06-93A8-D55B264E447D}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -988,13 +1104,14 @@
   <cols>
     <col min="2" max="2" width="20.140625" customWidth="1"/>
     <col min="3" max="3" width="22.85546875" customWidth="1"/>
-    <col min="6" max="6" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.85546875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1011,19 +1128,22 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G1" t="s">
         <v>16</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>71</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>18</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>49</v>
       </c>
@@ -1040,15 +1160,18 @@
         <v>4.49</v>
       </c>
       <c r="F2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2" t="s">
         <v>52</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>6</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>53</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>6</v>
       </c>
     </row>
@@ -1057,20 +1180,21 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CFF05D2F-E74C-42D4-9571-91DC8E544298}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="30" customWidth="1"/>
-    <col min="4" max="4" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1081,13 +1205,16 @@
         <v>4</v>
       </c>
       <c r="D1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E1" t="s">
         <v>25</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>64</v>
       </c>
@@ -1098,13 +1225,16 @@
         <v>63</v>
       </c>
       <c r="D2" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" t="s">
         <v>62</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>67</v>
       </c>
@@ -1115,13 +1245,16 @@
         <v>66</v>
       </c>
       <c r="D3" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" t="s">
         <v>59</v>
       </c>
-      <c r="E3" t="s">
+      <c r="F3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>48</v>
       </c>
@@ -1132,13 +1265,16 @@
         <v>68</v>
       </c>
       <c r="D4" t="s">
+        <v>48</v>
+      </c>
+      <c r="E4" t="s">
         <v>53</v>
       </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>48</v>
       </c>
@@ -1149,13 +1285,16 @@
         <v>68</v>
       </c>
       <c r="D5" t="s">
+        <v>48</v>
+      </c>
+      <c r="E5" t="s">
         <v>53</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>48</v>
       </c>
@@ -1166,9 +1305,12 @@
         <v>68</v>
       </c>
       <c r="D6" t="s">
+        <v>48</v>
+      </c>
+      <c r="E6" t="s">
         <v>47</v>
       </c>
-      <c r="E6" t="s">
+      <c r="F6" t="s">
         <v>30</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updates for InfluxDBProfiles, QuantityAndUnits, Sectors, random attributes
</commit_message>
<xml_diff>
--- a/data/infrastructure.xlsx
+++ b/data/infrastructure.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matthijssenef\PycharmProjects\excel-2-esdl\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88B4C749-824A-4F6F-B7A1-F2143CBDD36F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{242797A4-0A78-4030-9325-A2CAFFF26639}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10680" yWindow="3435" windowWidth="38700" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="51840" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Areas" sheetId="6" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="80">
   <si>
     <t>ID</t>
   </si>
@@ -75,12 +75,6 @@
     <t>Power</t>
   </si>
   <si>
-    <t>Efficiency_value</t>
-  </si>
-  <si>
-    <t>Efficiency_attribute</t>
-  </si>
-  <si>
     <t>InPort1_ID</t>
   </si>
   <si>
@@ -265,6 +259,18 @@
   </si>
   <si>
     <t>Area_WKT</t>
+  </si>
+  <si>
+    <t>Attribute1</t>
+  </si>
+  <si>
+    <t>Value1</t>
+  </si>
+  <si>
+    <t>Profile_Physical_Quantity</t>
+  </si>
+  <si>
+    <t>ENERGY</t>
   </si>
 </sst>
 </file>
@@ -603,16 +609,16 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D1" t="s">
+        <v>71</v>
+      </c>
+      <c r="E1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F1" t="s">
         <v>75</v>
-      </c>
-      <c r="D1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E1" t="s">
-        <v>74</v>
-      </c>
-      <c r="F1" t="s">
-        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -649,7 +655,7 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
   </sheetData>
@@ -704,13 +710,13 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B4" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C4" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -720,7 +726,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -734,11 +740,12 @@
     <col min="9" max="9" width="11.7109375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="9.85546875" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="13.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="11.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.5703125" customWidth="1"/>
+    <col min="13" max="13" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="11.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -755,39 +762,42 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G1" t="s">
         <v>13</v>
       </c>
       <c r="H1" t="s">
+        <v>18</v>
+      </c>
+      <c r="I1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K1" t="s">
+        <v>22</v>
+      </c>
+      <c r="L1" t="s">
+        <v>78</v>
+      </c>
+      <c r="M1" t="s">
         <v>20</v>
       </c>
-      <c r="I1" t="s">
-        <v>69</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="N1" t="s">
         <v>21</v>
       </c>
-      <c r="K1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L1" t="s">
-        <v>22</v>
-      </c>
-      <c r="M1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" t="s">
         <v>27</v>
       </c>
-      <c r="B2" t="s">
-        <v>29</v>
-      </c>
       <c r="C2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D2">
         <v>52.11</v>
@@ -796,39 +806,42 @@
         <v>4.51</v>
       </c>
       <c r="F2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G2">
         <v>10000</v>
       </c>
       <c r="H2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="I2" t="s">
+        <v>31</v>
+      </c>
+      <c r="J2" t="s">
         <v>33</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
+        <v>32</v>
+      </c>
+      <c r="L2" t="s">
+        <v>79</v>
+      </c>
+      <c r="M2">
+        <v>50</v>
+      </c>
+      <c r="N2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
         <v>35</v>
       </c>
-      <c r="K2" t="s">
-        <v>34</v>
-      </c>
-      <c r="L2">
-        <v>50</v>
-      </c>
-      <c r="M2" t="s">
+      <c r="B3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C3" t="s">
         <v>36</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B3" t="s">
-        <v>39</v>
-      </c>
-      <c r="C3" t="s">
-        <v>38</v>
       </c>
       <c r="D3">
         <v>52.104999999999997</v>
@@ -837,39 +850,42 @@
         <v>4.51</v>
       </c>
       <c r="F3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G3">
         <v>10000</v>
       </c>
       <c r="H3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="I3" t="s">
         <v>6</v>
       </c>
       <c r="J3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="K3" t="s">
+        <v>32</v>
+      </c>
+      <c r="L3" t="s">
+        <v>79</v>
+      </c>
+      <c r="M3">
+        <v>20</v>
+      </c>
+      <c r="N3" t="s">
         <v>34</v>
       </c>
-      <c r="L3">
-        <v>20</v>
-      </c>
-      <c r="M3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B4" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D4">
         <v>52.104999999999997</v>
@@ -878,32 +894,33 @@
         <v>4.47</v>
       </c>
       <c r="F4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G4" s="1">
         <v>1000000000</v>
       </c>
       <c r="H4" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I4" t="s">
         <v>7</v>
       </c>
       <c r="J4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="K4" t="s">
-        <v>48</v>
-      </c>
-      <c r="L4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="M4" t="s">
-        <v>48</v>
+        <v>46</v>
+      </c>
+      <c r="N4" t="s">
+        <v>46</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -947,37 +964,37 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G1" t="s">
         <v>13</v>
       </c>
       <c r="H1" t="s">
+        <v>76</v>
+      </c>
+      <c r="I1" t="s">
+        <v>77</v>
+      </c>
+      <c r="J1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" t="s">
+        <v>69</v>
+      </c>
+      <c r="L1" t="s">
         <v>15</v>
       </c>
-      <c r="I1" t="s">
-        <v>14</v>
-      </c>
-      <c r="J1" t="s">
+      <c r="M1" t="s">
+        <v>70</v>
+      </c>
+      <c r="N1" t="s">
         <v>16</v>
-      </c>
-      <c r="K1" t="s">
-        <v>71</v>
-      </c>
-      <c r="L1" t="s">
-        <v>17</v>
-      </c>
-      <c r="M1" t="s">
-        <v>72</v>
-      </c>
-      <c r="N1" t="s">
-        <v>18</v>
       </c>
       <c r="O1" t="s">
         <v>11</v>
       </c>
       <c r="P1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="Q1" t="s">
         <v>12</v>
@@ -985,13 +1002,13 @@
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" t="s">
         <v>42</v>
-      </c>
-      <c r="B2" t="s">
-        <v>43</v>
-      </c>
-      <c r="C2" t="s">
-        <v>44</v>
       </c>
       <c r="D2">
         <v>52.11</v>
@@ -1000,51 +1017,51 @@
         <v>4.5</v>
       </c>
       <c r="F2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G2">
         <v>4000</v>
       </c>
       <c r="H2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="I2">
         <v>3.2</v>
       </c>
       <c r="J2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="K2" t="s">
         <v>6</v>
       </c>
       <c r="L2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="M2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="N2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="O2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="P2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="Q2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" t="s">
         <v>54</v>
-      </c>
-      <c r="B3" t="s">
-        <v>55</v>
-      </c>
-      <c r="C3" t="s">
-        <v>56</v>
       </c>
       <c r="D3">
         <v>52.104999999999997</v>
@@ -1053,40 +1070,40 @@
         <v>4.4800000000000004</v>
       </c>
       <c r="F3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G3" s="1">
         <v>1000000000</v>
       </c>
       <c r="H3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="I3">
         <v>0.4</v>
       </c>
       <c r="J3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="K3" t="s">
         <v>7</v>
       </c>
       <c r="L3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="M3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="N3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="O3" t="s">
         <v>6</v>
       </c>
       <c r="P3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="Q3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
@@ -1128,16 +1145,16 @@
         <v>3</v>
       </c>
       <c r="F1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="G1" t="s">
+        <v>14</v>
+      </c>
+      <c r="H1" t="s">
+        <v>69</v>
+      </c>
+      <c r="I1" t="s">
         <v>16</v>
-      </c>
-      <c r="H1" t="s">
-        <v>71</v>
-      </c>
-      <c r="I1" t="s">
-        <v>18</v>
       </c>
       <c r="J1" t="s">
         <v>11</v>
@@ -1145,13 +1162,13 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" t="s">
         <v>49</v>
-      </c>
-      <c r="B2" t="s">
-        <v>50</v>
-      </c>
-      <c r="C2" t="s">
-        <v>51</v>
       </c>
       <c r="D2">
         <v>52.104999999999997</v>
@@ -1160,16 +1177,16 @@
         <v>4.49</v>
       </c>
       <c r="F2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="G2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H2" t="s">
         <v>6</v>
       </c>
       <c r="I2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="J2" t="s">
         <v>6</v>
@@ -1205,113 +1222,113 @@
         <v>4</v>
       </c>
       <c r="D1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C2" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D4" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E4" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F4" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D5" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E5" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C6" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D6" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
     </row>
   </sheetData>

</xml_diff>